<commit_message>
Reduce vm0 (aka Vcmax)
Canopy CO2 error was stemming from ridiculously high GPP drawing all of
the CO2 out of the canopy; reduce vm0 for PFT 8 (late pine/hemlock)
</commit_message>
<xml_diff>
--- a/PFT_Parameterizations.xlsx
+++ b/PFT_Parameterizations.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23900" windowHeight="28260" tabRatio="853"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="853" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="5 - Temp C3 Grass" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="77">
   <si>
     <t>Param</t>
   </si>
@@ -249,6 +249,12 @@
   </si>
   <si>
     <t>q -- fine root: leaf ratio</t>
+  </si>
+  <si>
+    <t>c2n_leaf (calculated)</t>
+  </si>
+  <si>
+    <t>qsw (calculated)</t>
   </si>
 </sst>
 </file>
@@ -327,8 +333,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="351">
+  <cellStyleXfs count="367">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -694,7 +716,7 @@
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="351">
+  <cellStyles count="367">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -870,6 +892,14 @@
     <cellStyle name="Followed Hyperlink" xfId="346" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="348" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="350" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="352" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="354" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="356" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="358" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="360" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="362" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="364" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="366" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1045,6 +1075,14 @@
     <cellStyle name="Hyperlink" xfId="345" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="347" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="349" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="351" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="353" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="355" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="357" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="359" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="361" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="363" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="365" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1376,7 +1414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -2082,8 +2120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView topLeftCell="A22" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2264,17 +2302,19 @@
         <v>43</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>56</v>
+        <v>76</v>
+      </c>
+      <c r="C10" s="2">
+        <f>C12/3900</f>
+        <v>1.5384615384615385E-3</v>
       </c>
       <c r="D10" s="2">
         <v>1.5384615E-3</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="5" t="s">
-        <v>66</v>
+      <c r="F10" s="2">
+        <f>F12/3900</f>
+        <v>3.0063025641025639E-3</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2312,8 +2352,7 @@
         <v>11.72458</v>
       </c>
       <c r="F12" s="2">
-        <f>D12</f>
-        <v>6</v>
+        <v>11.72458</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2348,7 +2387,7 @@
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="2">
-        <f>D14</f>
+        <f t="shared" ref="F14:F21" si="1">D14</f>
         <v>0</v>
       </c>
     </row>
@@ -2366,7 +2405,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="2">
-        <f>D15</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2384,7 +2423,7 @@
         <v>20</v>
       </c>
       <c r="F16" s="2">
-        <f>D16</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
     </row>
@@ -2402,7 +2441,7 @@
         <v>3.3928000000000001E-3</v>
       </c>
       <c r="F17" s="2">
-        <f>D17</f>
+        <f t="shared" si="1"/>
         <v>3.3928000000000001E-3</v>
       </c>
     </row>
@@ -2424,7 +2463,7 @@
         <v>192</v>
       </c>
       <c r="F18" s="2">
-        <f>D18</f>
+        <f t="shared" si="1"/>
         <v>193</v>
       </c>
     </row>
@@ -2442,7 +2481,7 @@
         <v>0.94999998809999997</v>
       </c>
       <c r="F19" s="2">
-        <f>D19</f>
+        <f t="shared" si="1"/>
         <v>0.94999998809999997</v>
       </c>
     </row>
@@ -2460,7 +2499,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="2">
-        <f>D20</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2478,7 +2517,7 @@
         <v>0.1000000015</v>
       </c>
       <c r="F21" s="2">
-        <f>D21</f>
+        <f t="shared" si="1"/>
         <v>0.1000000015</v>
       </c>
     </row>
@@ -2487,10 +2526,11 @@
         <v>54</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>56</v>
+        <v>75</v>
+      </c>
+      <c r="C22" s="9">
+        <f>1000/((0.11289+0.12947*15.625)*C12)</f>
+        <v>78.032625831023083</v>
       </c>
       <c r="D22" s="9">
         <v>78.032623290999993</v>
@@ -2498,8 +2538,9 @@
       <c r="E22" s="9">
         <v>39.463999999999999</v>
       </c>
-      <c r="F22" s="5" t="s">
-        <v>66</v>
+      <c r="F22" s="7">
+        <f>1000/((0.11289+0.12947*15.625)*F12)</f>
+        <v>39.932838104745628</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>67</v>
@@ -2519,9 +2560,8 @@
         <v>1000</v>
       </c>
       <c r="E23" s="9"/>
-      <c r="F23" s="9">
-        <f>D23</f>
-        <v>1000</v>
+      <c r="F23" s="5">
+        <v>2000</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -2538,7 +2578,7 @@
         <v>9.9999997999999993E-3</v>
       </c>
       <c r="F24" s="2">
-        <f>D24</f>
+        <f t="shared" ref="F24:F30" si="2">D24</f>
         <v>9.9999997999999993E-3</v>
       </c>
     </row>
@@ -2556,7 +2596,7 @@
         <v>1.9999999599999999E-2</v>
       </c>
       <c r="F25" s="2">
-        <f>D25</f>
+        <f t="shared" si="2"/>
         <v>1.9999999599999999E-2</v>
       </c>
     </row>
@@ -2574,7 +2614,7 @@
         <v>5.0000000699999998E-2</v>
       </c>
       <c r="F26" s="2">
-        <f>D26</f>
+        <f t="shared" si="2"/>
         <v>5.0000000699999998E-2</v>
       </c>
     </row>
@@ -2593,7 +2633,7 @@
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="2">
-        <f>D27</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
@@ -2614,7 +2654,7 @@
         <v>5.8105999999999998E-2</v>
       </c>
       <c r="F28" s="2">
-        <f>D28</f>
+        <f t="shared" si="2"/>
         <v>7.9999998200000005E-2</v>
       </c>
     </row>
@@ -2632,7 +2672,7 @@
         <v>6.3948998451000003</v>
       </c>
       <c r="F29" s="2">
-        <f>D29</f>
+        <f t="shared" si="2"/>
         <v>6.3948998451000003</v>
       </c>
     </row>
@@ -2650,7 +2690,7 @@
         <v>4.7136998177000002</v>
       </c>
       <c r="F30" s="2">
-        <f>D30</f>
+        <f t="shared" si="2"/>
         <v>4.7136998177000002</v>
       </c>
     </row>
@@ -2671,7 +2711,7 @@
         <v>36.388370000000002</v>
       </c>
       <c r="F31" s="5">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>68</v>
@@ -2781,7 +2821,7 @@
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2">
-        <f>D37</f>
+        <f t="shared" ref="F37:F43" si="3">D37</f>
         <v>0.76599997279999998</v>
       </c>
     </row>
@@ -2799,7 +2839,7 @@
         <v>0.30000001189999997</v>
       </c>
       <c r="F38" s="2">
-        <f>D38</f>
+        <f t="shared" si="3"/>
         <v>0.30000001189999997</v>
       </c>
     </row>
@@ -2817,7 +2857,7 @@
         <v>5</v>
       </c>
       <c r="F39" s="2">
-        <f>D39</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
     </row>
@@ -2835,7 +2875,7 @@
         <v>0.05</v>
       </c>
       <c r="F40" s="2">
-        <f>D40</f>
+        <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
     </row>
@@ -2853,7 +2893,7 @@
         <v>0.79000002150000004</v>
       </c>
       <c r="F41" s="2">
-        <f>D41</f>
+        <f t="shared" si="3"/>
         <v>0.79000002150000004</v>
       </c>
     </row>
@@ -2871,7 +2911,7 @@
         <v>0.45030000809999998</v>
       </c>
       <c r="F42" s="2">
-        <f>D42</f>
+        <f t="shared" si="3"/>
         <v>0.45030000809999998</v>
       </c>
     </row>
@@ -2892,7 +2932,7 @@
         <v>0.3276</v>
       </c>
       <c r="F43" s="2">
-        <f>D43</f>
+        <f t="shared" si="3"/>
         <v>0.33300000429999999</v>
       </c>
     </row>
@@ -2984,8 +3024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:F32"/>
+    <sheetView topLeftCell="A23" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3166,17 +3206,19 @@
         <v>43</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>56</v>
+        <v>76</v>
+      </c>
+      <c r="C10" s="2">
+        <f>C12/3900</f>
+        <v>2.5641025641025641E-3</v>
       </c>
       <c r="D10" s="2">
         <v>2.5641026000000002E-3</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="5" t="s">
-        <v>66</v>
+      <c r="F10" s="2">
+        <f>F12/3900</f>
+        <v>2.7457256410256411E-3</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -3213,8 +3255,8 @@
       <c r="E12" s="2">
         <v>10.70833</v>
       </c>
-      <c r="F12" s="7">
-        <v>10.7</v>
+      <c r="F12" s="2">
+        <v>10.70833</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -3387,16 +3429,18 @@
         <v>54</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>56</v>
+        <v>75</v>
+      </c>
+      <c r="C22" s="2">
+        <f>1000/((0.11289+0.12947*6.25)*C12)</f>
+        <v>108.45075386830281</v>
       </c>
       <c r="D22" s="2">
         <v>108.4507446289</v>
       </c>
-      <c r="F22" s="5" t="s">
-        <v>66</v>
+      <c r="F22" s="2">
+        <f>1000/((0.11289+0.12947*6.25)*F12)</f>
+        <v>101.27700011888206</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -3413,9 +3457,8 @@
         <v>1000</v>
       </c>
       <c r="E23" s="7"/>
-      <c r="F23" s="7">
-        <f>D23</f>
-        <v>1000</v>
+      <c r="F23" s="5">
+        <v>2000</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -3432,7 +3475,7 @@
         <v>9.9999997999999993E-3</v>
       </c>
       <c r="F24" s="2">
-        <f>D24</f>
+        <f t="shared" ref="F24:F30" si="1">D24</f>
         <v>9.9999997999999993E-3</v>
       </c>
     </row>
@@ -3450,7 +3493,7 @@
         <v>1.9999999599999999E-2</v>
       </c>
       <c r="F25" s="2">
-        <f>D25</f>
+        <f t="shared" si="1"/>
         <v>1.9999999599999999E-2</v>
       </c>
     </row>
@@ -3468,7 +3511,7 @@
         <v>5.0000000699999998E-2</v>
       </c>
       <c r="F26" s="2">
-        <f>D26</f>
+        <f t="shared" si="1"/>
         <v>5.0000000699999998E-2</v>
       </c>
     </row>
@@ -3487,7 +3530,7 @@
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="2">
-        <f>D27</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
@@ -3508,7 +3551,7 @@
         <v>7.3050000000000004E-2</v>
       </c>
       <c r="F28" s="2">
-        <f>D28</f>
+        <f t="shared" si="1"/>
         <v>7.9999998200000005E-2</v>
       </c>
     </row>
@@ -3526,7 +3569,7 @@
         <v>6.3948998451000003</v>
       </c>
       <c r="F29" s="2">
-        <f>D29</f>
+        <f t="shared" si="1"/>
         <v>6.3948998451000003</v>
       </c>
     </row>
@@ -3544,7 +3587,7 @@
         <v>4.7136998177000002</v>
       </c>
       <c r="F30" s="2">
-        <f>D30</f>
+        <f t="shared" si="1"/>
         <v>4.7136998177000002</v>
       </c>
     </row>
@@ -3564,8 +3607,8 @@
       <c r="E31" s="9">
         <v>72.380390000000006</v>
       </c>
-      <c r="F31" s="5" t="s">
-        <v>66</v>
+      <c r="F31" s="5">
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -3672,7 +3715,7 @@
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2">
-        <f>D37</f>
+        <f t="shared" ref="F37:F43" si="2">D37</f>
         <v>1E-3</v>
       </c>
     </row>
@@ -3690,7 +3733,7 @@
         <v>0.30000001189999997</v>
       </c>
       <c r="F38" s="2">
-        <f>D38</f>
+        <f t="shared" si="2"/>
         <v>0.30000001189999997</v>
       </c>
     </row>
@@ -3708,7 +3751,7 @@
         <v>5</v>
       </c>
       <c r="F39" s="2">
-        <f>D39</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
     </row>
@@ -3726,7 +3769,7 @@
         <v>0.5</v>
       </c>
       <c r="F40" s="2">
-        <f>D40</f>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
     </row>
@@ -3744,7 +3787,7 @@
         <v>0.79000002150000004</v>
       </c>
       <c r="F41" s="2">
-        <f>D41</f>
+        <f t="shared" si="2"/>
         <v>0.79000002150000004</v>
       </c>
     </row>
@@ -3762,7 +3805,7 @@
         <v>0.45030000809999998</v>
       </c>
       <c r="F42" s="2">
-        <f>D42</f>
+        <f t="shared" si="2"/>
         <v>0.45030000809999998</v>
       </c>
     </row>
@@ -3780,7 +3823,7 @@
         <v>0.33300000429999999</v>
       </c>
       <c r="F43" s="2">
-        <f>D43</f>
+        <f t="shared" si="2"/>
         <v>0.33300000429999999</v>
       </c>
     </row>
@@ -3868,8 +3911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView topLeftCell="A23" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4055,17 +4098,19 @@
         <v>43</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>56</v>
+        <v>76</v>
+      </c>
+      <c r="C10" s="2">
+        <f>C12/3900</f>
+        <v>7.6923076923076927E-3</v>
       </c>
       <c r="D10" s="2">
         <v>7.6923076999999996E-3</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="5" t="s">
-        <v>66</v>
+      <c r="F10" s="2">
+        <f>F12/3900</f>
+        <v>7.6923076923076927E-3</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -4277,10 +4322,11 @@
         <v>54</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>56</v>
+        <v>75</v>
+      </c>
+      <c r="C22" s="2">
+        <f>1000/((0.11289+0.12947*18.25)*C12)</f>
+        <v>13.464110236056147</v>
       </c>
       <c r="D22" s="2">
         <v>13.4641094208</v>
@@ -4288,8 +4334,9 @@
       <c r="E22" s="2">
         <v>19.681000000000001</v>
       </c>
-      <c r="F22" s="5" t="s">
-        <v>66</v>
+      <c r="F22" s="2">
+        <f>1000/((0.11289+0.12947*18.25)*F12)</f>
+        <v>13.464110236056147</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -4306,7 +4353,7 @@
         <v>20000</v>
       </c>
       <c r="E23" s="9"/>
-      <c r="F23" s="5">
+      <c r="F23" s="7">
         <v>10000</v>
       </c>
     </row>
@@ -4344,9 +4391,8 @@
       <c r="E25" s="2">
         <v>1.9126339999999999E-2</v>
       </c>
-      <c r="F25" s="2">
-        <f t="shared" si="0"/>
-        <v>3.3985305600000001E-2</v>
+      <c r="F25" s="5">
+        <v>1.9130000000000001E-2</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -4462,8 +4508,8 @@
       <c r="E31" s="9">
         <v>56.31326</v>
       </c>
-      <c r="F31" s="5" t="s">
-        <v>66</v>
+      <c r="F31" s="5">
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -4772,8 +4818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView topLeftCell="A23" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4959,17 +5005,19 @@
         <v>43</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>56</v>
+        <v>76</v>
+      </c>
+      <c r="C10" s="2">
+        <f>C12/3900</f>
+        <v>6.2051282051282051E-3</v>
       </c>
       <c r="D10" s="2">
         <v>6.2051284999999996E-3</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="5" t="s">
-        <v>66</v>
+      <c r="F10" s="2">
+        <f>F12/3900</f>
+        <v>7.6504394335641024E-3</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -5182,16 +5230,18 @@
         <v>54</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>56</v>
+        <v>75</v>
+      </c>
+      <c r="C22" s="2">
+        <f>1000/((0.11289+0.12947*15.625)*C12)</f>
+        <v>19.3469320242206</v>
       </c>
       <c r="D22" s="2">
         <v>19.346931457499998</v>
       </c>
-      <c r="F22" s="5" t="s">
-        <v>66</v>
+      <c r="F22" s="2">
+        <f>1000/((0.11289+0.12947*15.625)*F12)</f>
+        <v>15.691934382161586</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -5208,7 +5258,7 @@
         <v>20000</v>
       </c>
       <c r="E23" s="9"/>
-      <c r="F23" s="5">
+      <c r="F23" s="7">
         <v>10000</v>
       </c>
     </row>
@@ -5361,8 +5411,8 @@
       <c r="E31" s="9">
         <v>37.854599999999998</v>
       </c>
-      <c r="F31" s="5" t="s">
-        <v>66</v>
+      <c r="F31" s="5">
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -5372,7 +5422,7 @@
       <c r="B32" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="7">
         <f>300/(365*24*60*60)</f>
         <v>9.5129375951293768E-6</v>
       </c>
@@ -5669,8 +5719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5856,17 +5906,19 @@
         <v>43</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>56</v>
+        <v>76</v>
+      </c>
+      <c r="C10" s="2">
+        <f>C12/3900</f>
+        <v>1.5384615384615385E-2</v>
       </c>
       <c r="D10" s="2">
         <v>1.5384615399999999E-2</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="5" t="s">
-        <v>66</v>
+      <c r="F10" s="2">
+        <f>F12/3900</f>
+        <v>1.0133104568871794E-2</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -6079,10 +6131,11 @@
         <v>54</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>56</v>
+        <v>75</v>
+      </c>
+      <c r="C22" s="2">
+        <f>1000/((0.11289+0.12947*6.25)*C12)</f>
+        <v>18.075125644717136</v>
       </c>
       <c r="D22" s="2">
         <v>18.0751247406</v>
@@ -6090,8 +6143,9 @@
       <c r="E22" s="2">
         <v>21.373000000000001</v>
       </c>
-      <c r="F22" s="5" t="s">
-        <v>66</v>
+      <c r="F22" s="2">
+        <f>1000/((0.11289+0.12947*6.25)*F12)</f>
+        <v>27.442611904628972</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -6108,7 +6162,7 @@
         <v>20000</v>
       </c>
       <c r="E23" s="9"/>
-      <c r="F23" s="5">
+      <c r="F23" s="7">
         <v>10000</v>
       </c>
     </row>
@@ -6264,8 +6318,8 @@
       <c r="E31" s="2">
         <v>69.785049999999998</v>
       </c>
-      <c r="F31" s="5" t="s">
-        <v>66</v>
+      <c r="F31" s="5">
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -6390,7 +6444,7 @@
         <v>0.31190443039999999</v>
       </c>
       <c r="F38" s="2">
-        <f>D38</f>
+        <f t="shared" ref="F38:F43" si="1">D38</f>
         <v>0.31190443039999999</v>
       </c>
     </row>
@@ -6408,7 +6462,7 @@
         <v>5</v>
       </c>
       <c r="F39" s="2">
-        <f>D39</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
@@ -6426,7 +6480,7 @@
         <v>0.05</v>
       </c>
       <c r="F40" s="2">
-        <f>D40</f>
+        <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
     </row>
@@ -6444,7 +6498,7 @@
         <v>0.79000002150000004</v>
       </c>
       <c r="F41" s="2">
-        <f>D41</f>
+        <f t="shared" si="1"/>
         <v>0.79000002150000004</v>
       </c>
     </row>
@@ -6462,7 +6516,7 @@
         <v>0.35075291990000002</v>
       </c>
       <c r="F42" s="2">
-        <f>D42</f>
+        <f t="shared" si="1"/>
         <v>0.35075291990000002</v>
       </c>
     </row>
@@ -6480,7 +6534,7 @@
         <v>0</v>
       </c>
       <c r="F43" s="2">
-        <f>D43</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Trying to fix composition
Some changes to PFTs and ED2IN setting trying to get more hardwoods on
the landscape.  Old parameterization had good biomass, but pretty much
only PFT 8 on the landscape
</commit_message>
<xml_diff>
--- a/PFT_Parameterizations.xlsx
+++ b/PFT_Parameterizations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="0" windowWidth="29240" windowHeight="27100" tabRatio="853" activeTab="5"/>
+    <workbookView xWindow="140" yWindow="0" windowWidth="29240" windowHeight="27100" tabRatio="853" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="5 - Temp C3 Grass" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="120">
   <si>
     <t>Param</t>
   </si>
@@ -370,6 +370,24 @@
   <si>
     <t>Kelly South Pine (Bety/Pecan)</t>
   </si>
+  <si>
+    <t xml:space="preserve">between mean-2sd late conifer &amp; general temperate conifer </t>
+  </si>
+  <si>
+    <t>mean + 2 SD</t>
+  </si>
+  <si>
+    <t>generic temp decid</t>
+  </si>
+  <si>
+    <t>made up to be more similar to conifers</t>
+  </si>
+  <si>
+    <t>from mid-hardwood</t>
+  </si>
+  <si>
+    <t>same as north pine</t>
+  </si>
 </sst>
 </file>
 
@@ -423,7 +441,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -492,12 +510,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2DCDB"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -518,7 +530,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1369">
+  <cellStyleXfs count="1371">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1888,8 +1900,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1912,12 +1926,11 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="4" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="4" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="4" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1369">
+  <cellStyles count="1371">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2602,6 +2615,7 @@
     <cellStyle name="Followed Hyperlink" xfId="1364" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1366" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1368" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1370" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3286,6 +3300,7 @@
     <cellStyle name="Hyperlink" xfId="1363" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1365" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1367" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1369" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4324,9 +4339,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I45" sqref="I45"/>
+      <selection pane="topRight" activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4692,7 +4707,7 @@
         <v>3.3928000000000001E-3</v>
       </c>
       <c r="H17" s="2">
-        <f t="shared" ref="H17:H29" si="3">C17</f>
+        <f t="shared" ref="H17:H27" si="3">C17</f>
         <v>3.3928000000000001E-3</v>
       </c>
     </row>
@@ -4819,7 +4834,7 @@
       <c r="E23" s="7">
         <v>4426.9797352549103</v>
       </c>
-      <c r="H23" s="23">
+      <c r="H23" s="22">
         <f>E23</f>
         <v>4426.9797352549103</v>
       </c>
@@ -4952,7 +4967,7 @@
       <c r="E29" s="7">
         <v>8.9086404610425198</v>
       </c>
-      <c r="H29" s="23">
+      <c r="H29" s="22">
         <f>E29</f>
         <v>8.9086404610425198</v>
       </c>
@@ -4973,7 +4988,7 @@
       <c r="E30" s="7">
         <v>5.0524412393947404</v>
       </c>
-      <c r="H30" s="23">
+      <c r="H30" s="22">
         <f>E30</f>
         <v>5.0524412393947404</v>
       </c>
@@ -5025,7 +5040,7 @@
       <c r="E32" s="7">
         <v>4.5659112777780304E-3</v>
       </c>
-      <c r="H32" s="25">
+      <c r="H32" s="24">
         <v>0.62139999999999995</v>
       </c>
     </row>
@@ -5117,7 +5132,7 @@
       </c>
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
-      <c r="H37" s="25">
+      <c r="H37" s="24">
         <v>0.62139999999999995</v>
       </c>
     </row>
@@ -5137,7 +5152,7 @@
       <c r="E38" s="7">
         <v>0.32102528456778301</v>
       </c>
-      <c r="H38" s="25">
+      <c r="H38" s="24">
         <v>0.62139999999999995</v>
       </c>
     </row>
@@ -5155,7 +5170,7 @@
         <v>5</v>
       </c>
       <c r="H39" s="2">
-        <f t="shared" ref="H38:H43" si="5">C39</f>
+        <f t="shared" ref="H39:H41" si="5">C39</f>
         <v>5</v>
       </c>
     </row>
@@ -5217,11 +5232,11 @@
       <c r="E42" s="7">
         <v>0.27140086835400401</v>
       </c>
-      <c r="H42" s="23">
+      <c r="H42" s="22">
         <f>E42</f>
         <v>0.27140086835400401</v>
       </c>
-      <c r="I42" s="23"/>
+      <c r="I42" s="22"/>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="7" t="s">
@@ -5294,7 +5309,7 @@
       <c r="E45" s="7">
         <v>0.62139806485750004</v>
       </c>
-      <c r="H45" s="23">
+      <c r="H45" s="22">
         <f>E45</f>
         <v>0.62139806485750004</v>
       </c>
@@ -5347,10 +5362,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A19" sqref="A19"/>
-      <selection pane="topRight" activeCell="I9" sqref="I9"/>
+      <selection pane="topRight" activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5536,7 +5551,7 @@
       <c r="E9" s="7">
         <v>0.76880331308720196</v>
       </c>
-      <c r="I9" s="23">
+      <c r="I9" s="22">
         <f>E9</f>
         <v>0.76880331308720196</v>
       </c>
@@ -5689,7 +5704,7 @@
       <c r="E16" s="7">
         <v>19.6430837553782</v>
       </c>
-      <c r="I16" s="23">
+      <c r="I16" s="22">
         <f>E16</f>
         <v>19.6430837553782</v>
       </c>
@@ -5746,7 +5761,7 @@
       <c r="E19" s="7">
         <v>0.94947512611457996</v>
       </c>
-      <c r="I19" s="23">
+      <c r="I19" s="22">
         <f>E19</f>
         <v>0.94947512611457996</v>
       </c>
@@ -5825,12 +5840,12 @@
       <c r="D23" s="7">
         <v>1000</v>
       </c>
-      <c r="I23" s="23">
-        <f>C23</f>
-        <v>1000</v>
+      <c r="I23" s="22">
+        <f>'6 - North Pine'!H23</f>
+        <v>4426.9797352549103</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -5888,7 +5903,7 @@
       <c r="E26" s="7">
         <v>0.101805307921965</v>
       </c>
-      <c r="I26" s="23">
+      <c r="I26" s="22">
         <f>E26</f>
         <v>0.101805307921965</v>
       </c>
@@ -5961,7 +5976,7 @@
       <c r="E29" s="7">
         <v>9.0244611720554495</v>
       </c>
-      <c r="I29" s="23">
+      <c r="I29" s="22">
         <f>E29</f>
         <v>9.0244611720554495</v>
       </c>
@@ -5982,7 +5997,7 @@
       <c r="E30" s="7">
         <v>5.0242533271584797</v>
       </c>
-      <c r="I30" s="23">
+      <c r="I30" s="22">
         <f>E30</f>
         <v>5.0242533271584797</v>
       </c>
@@ -6010,8 +6025,10 @@
         <v>72.380390000000006</v>
       </c>
       <c r="I31" s="16">
-        <f>H31</f>
-        <v>72.380390000000006</v>
+        <v>50</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -6031,7 +6048,7 @@
       <c r="E32" s="7">
         <v>4.4835993117889996E-3</v>
       </c>
-      <c r="I32" s="23">
+      <c r="I32" s="22">
         <f>E32</f>
         <v>4.4835993117889996E-3</v>
       </c>
@@ -6130,7 +6147,7 @@
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
-      <c r="I37" s="23">
+      <c r="I37" s="22">
         <f>E37</f>
         <v>0.39221339141122002</v>
       </c>
@@ -6151,7 +6168,7 @@
       <c r="E38" s="7">
         <v>0.31896799063861297</v>
       </c>
-      <c r="I38" s="23">
+      <c r="I38" s="22">
         <f>E38</f>
         <v>0.31896799063861297</v>
       </c>
@@ -6211,7 +6228,7 @@
       <c r="E41" s="7">
         <v>0.50661508232696595</v>
       </c>
-      <c r="I41" s="23">
+      <c r="I41" s="22">
         <f>E41</f>
         <v>0.50661508232696595</v>
       </c>
@@ -6232,11 +6249,11 @@
       <c r="E42" s="7">
         <v>0.27136302697237402</v>
       </c>
-      <c r="I42" s="23">
+      <c r="I42" s="22">
         <f>E42</f>
         <v>0.27136302697237402</v>
       </c>
-      <c r="J42" s="23" t="s">
+      <c r="J42" s="22" t="s">
         <v>103</v>
       </c>
     </row>
@@ -6372,7 +6389,7 @@
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A19" sqref="A19"/>
-      <selection pane="topRight" activeCell="K13" sqref="K13"/>
+      <selection pane="topRight" activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6381,14 +6398,14 @@
     <col min="2" max="2" width="26.33203125" style="7" customWidth="1"/>
     <col min="3" max="3" width="9.5" style="7" customWidth="1"/>
     <col min="4" max="5" width="13" style="7" customWidth="1"/>
-    <col min="6" max="6" width="13" style="24" customWidth="1"/>
+    <col min="6" max="6" width="13" style="23" customWidth="1"/>
     <col min="7" max="7" width="9.1640625" style="7" customWidth="1"/>
     <col min="8" max="10" width="10.83203125" style="7" customWidth="1"/>
     <col min="11" max="11" width="11.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1">
+    <row r="1" spans="1:12" s="1" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>41</v>
       </c>
@@ -6423,7 +6440,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:12">
       <c r="A2" s="7" t="s">
         <v>42</v>
       </c>
@@ -6441,7 +6458,7 @@
         <v>1.29E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:12">
       <c r="A3" s="7" t="s">
         <v>42</v>
       </c>
@@ -6459,7 +6476,7 @@
         <v>2.648E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:12">
       <c r="A4" s="7" t="s">
         <v>42</v>
       </c>
@@ -6477,7 +6494,7 @@
         <v>22.6799</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:12">
       <c r="A5" s="7" t="s">
         <v>42</v>
       </c>
@@ -6495,7 +6512,7 @@
         <v>1.7477</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:12">
       <c r="A6" s="7" t="s">
         <v>42</v>
       </c>
@@ -6513,7 +6530,7 @@
         <v>2.9595400000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:12">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -6531,7 +6548,7 @@
         <v>-6.5339999999999995E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:12">
       <c r="A8" s="7" t="s">
         <v>42</v>
       </c>
@@ -6549,7 +6566,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:12">
       <c r="A9" s="7" t="s">
         <v>42</v>
       </c>
@@ -6565,7 +6582,7 @@
       <c r="E9" s="7">
         <v>0.63578678943003997</v>
       </c>
-      <c r="F9" s="24">
+      <c r="F9" s="23">
         <v>0.63596261938961296</v>
       </c>
       <c r="G9" s="7">
@@ -6585,7 +6602,7 @@
         <v>0.63580000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="3" customFormat="1">
+    <row r="10" spans="1:12" s="3" customFormat="1">
       <c r="A10" s="7" t="s">
         <v>42</v>
       </c>
@@ -6600,17 +6617,19 @@
         <v>7.6923076999999996E-3</v>
       </c>
       <c r="E10" s="7"/>
-      <c r="F10" s="24"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
       <c r="K10" s="13">
-        <f>K12/3900</f>
-        <v>1.097478717948718E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="7" t="s">
         <v>42</v>
       </c>
@@ -6628,7 +6647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:12">
       <c r="A12" s="7" t="s">
         <v>42</v>
       </c>
@@ -6644,7 +6663,7 @@
       <c r="E12" s="7">
         <v>28.460754447603101</v>
       </c>
-      <c r="F12" s="24">
+      <c r="F12" s="23">
         <v>42.799007023340998</v>
       </c>
       <c r="G12" s="7">
@@ -6664,7 +6683,7 @@
         <v>42.801670000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:12">
       <c r="A13" s="7" t="s">
         <v>54</v>
       </c>
@@ -6682,7 +6701,7 @@
         <v>calculated</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:12">
       <c r="A14" s="8" t="s">
         <v>44</v>
       </c>
@@ -6705,7 +6724,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:12">
       <c r="A15" s="7" t="s">
         <v>49</v>
       </c>
@@ -6723,7 +6742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:12">
       <c r="A16" s="7" t="s">
         <v>49</v>
       </c>
@@ -6736,10 +6755,10 @@
       <c r="D16" s="7">
         <v>20</v>
       </c>
-      <c r="F16" s="24">
+      <c r="F16" s="23">
         <v>43.108631057548301</v>
       </c>
-      <c r="K16" s="23">
+      <c r="K16" s="22">
         <f>F16</f>
         <v>43.108631057548301</v>
       </c>
@@ -6794,10 +6813,10 @@
       <c r="D19" s="7">
         <v>0.94999998809999997</v>
       </c>
-      <c r="F19" s="24">
+      <c r="F19" s="23">
         <v>0.947713780677375</v>
       </c>
-      <c r="K19" s="23">
+      <c r="K19" s="22">
         <f>F19</f>
         <v>0.947713780677375</v>
       </c>
@@ -6852,7 +6871,7 @@
       <c r="D22" s="7">
         <v>13.4641094208</v>
       </c>
-      <c r="F22" s="24">
+      <c r="F22" s="23">
         <v>19.680132766755001</v>
       </c>
       <c r="G22" s="7">
@@ -6879,11 +6898,13 @@
       <c r="D23" s="7">
         <v>20000</v>
       </c>
-      <c r="K23" s="23">
-        <f>C23</f>
-        <v>10000</v>
-      </c>
-      <c r="L23" s="4"/>
+      <c r="K23" s="22">
+        <f>'10 -  Mid Hardwood'!K23</f>
+        <v>7904</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="11" t="s">
@@ -6922,7 +6943,7 @@
       <c r="E25" s="7">
         <v>3.39853068703957E-2</v>
       </c>
-      <c r="F25" s="24">
+      <c r="F25" s="23">
         <v>1.9126424044692301E-2</v>
       </c>
       <c r="G25" s="7">
@@ -6955,10 +6976,10 @@
       <c r="D26" s="7">
         <v>5.0000000699999998E-2</v>
       </c>
-      <c r="F26" s="24">
+      <c r="F26" s="23">
         <v>0.101006790121505</v>
       </c>
-      <c r="K26" s="23">
+      <c r="K26" s="22">
         <f>F26</f>
         <v>0.101006790121505</v>
       </c>
@@ -7002,7 +7023,7 @@
       <c r="E28" s="7">
         <v>5.7775914219179998E-2</v>
       </c>
-      <c r="F28" s="24">
+      <c r="F28" s="23">
         <v>5.73388436893933E-2</v>
       </c>
       <c r="G28" s="7">
@@ -7038,7 +7059,7 @@
       <c r="E29" s="7">
         <v>5.8748330304446501</v>
       </c>
-      <c r="F29" s="24">
+      <c r="F29" s="23">
         <v>6.1731631374525104</v>
       </c>
       <c r="G29" s="7">
@@ -7071,10 +7092,10 @@
       <c r="D30" s="7">
         <v>4.7136998177000002</v>
       </c>
-      <c r="F30" s="24">
+      <c r="F30" s="23">
         <v>4.98546861532368</v>
       </c>
-      <c r="K30" s="23">
+      <c r="K30" s="22">
         <f>F30</f>
         <v>4.98546861532368</v>
       </c>
@@ -7095,7 +7116,7 @@
       <c r="E31" s="7">
         <v>27.960888738123401</v>
       </c>
-      <c r="F31" s="24">
+      <c r="F31" s="23">
         <v>56.316556547444598</v>
       </c>
       <c r="G31" s="7">
@@ -7111,8 +7132,10 @@
         <v>56.289279999999998</v>
       </c>
       <c r="K31" s="2">
-        <f>I31</f>
-        <v>56.31326</v>
+        <v>57.3</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -7132,10 +7155,10 @@
       <c r="E32" s="7">
         <v>4.9651669160430296E-3</v>
       </c>
-      <c r="F32" s="24">
+      <c r="F32" s="23">
         <v>4.2579909421441697E-3</v>
       </c>
-      <c r="K32" s="23">
+      <c r="K32" s="22">
         <f>F32</f>
         <v>4.2579909421441697E-3</v>
       </c>
@@ -7175,7 +7198,7 @@
         <v>7.4074082099999994E-2</v>
       </c>
       <c r="K34" s="2" t="str">
-        <f t="shared" ref="K32:K41" si="2">C34</f>
+        <f t="shared" ref="K34:K39" si="2">C34</f>
         <v>calculated</v>
       </c>
     </row>
@@ -7229,14 +7252,14 @@
         <v>1</v>
       </c>
       <c r="E37" s="7"/>
-      <c r="F37" s="24">
+      <c r="F37" s="23">
         <v>0.41756016771510801</v>
       </c>
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
-      <c r="K37" s="23">
+      <c r="K37" s="22">
         <f>F37</f>
         <v>0.41756016771510801</v>
       </c>
@@ -7257,10 +7280,10 @@
       <c r="E38" s="7">
         <v>0.318077268126368</v>
       </c>
-      <c r="F38" s="24">
+      <c r="F38" s="23">
         <v>0.31256999133930702</v>
       </c>
-      <c r="K38" s="23">
+      <c r="K38" s="22">
         <f>F38</f>
         <v>0.31256999133930702</v>
       </c>
@@ -7317,10 +7340,10 @@
       <c r="D41" s="7">
         <v>0.79000002150000004</v>
       </c>
-      <c r="F41" s="24">
+      <c r="F41" s="23">
         <v>0.49579110420655098</v>
       </c>
-      <c r="K41" s="23">
+      <c r="K41" s="22">
         <f>F41</f>
         <v>0.49579110420655098</v>
       </c>
@@ -7341,14 +7364,14 @@
       <c r="E42" s="7">
         <v>0.35128400542426502</v>
       </c>
-      <c r="F42" s="24">
+      <c r="F42" s="23">
         <v>0.35321762744686103</v>
       </c>
-      <c r="K42" s="23">
+      <c r="K42" s="22">
         <f>F42</f>
         <v>0.35321762744686103</v>
       </c>
-      <c r="L42" s="23"/>
+      <c r="L42" s="22"/>
     </row>
     <row r="43" spans="1:12">
       <c r="A43" s="7" t="s">
@@ -7385,7 +7408,7 @@
       <c r="E44" s="7">
         <v>2.9454385969416799</v>
       </c>
-      <c r="F44" s="24">
+      <c r="F44" s="23">
         <v>1.45245938057048</v>
       </c>
       <c r="G44" s="7">
@@ -7423,7 +7446,7 @@
       <c r="E45" s="7">
         <v>0.69149308155026701</v>
       </c>
-      <c r="F45" s="24">
+      <c r="F45" s="23">
         <v>1.2992295068411901</v>
       </c>
       <c r="G45" s="7">
@@ -7438,7 +7461,7 @@
       <c r="J45" s="7">
         <v>1.2782</v>
       </c>
-      <c r="K45" s="23">
+      <c r="K45" s="22">
         <v>0.7</v>
       </c>
     </row>
@@ -7455,7 +7478,7 @@
       <c r="D46" s="7">
         <v>0</v>
       </c>
-      <c r="F46" s="24">
+      <c r="F46" s="23">
         <v>0</v>
       </c>
       <c r="K46" s="17">
@@ -7517,7 +7540,7 @@
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A19" sqref="A19"/>
-      <selection pane="topRight" activeCell="F45" sqref="F45"/>
+      <selection pane="topRight" activeCell="K10" sqref="K10:L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7534,7 +7557,7 @@
     <col min="12" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1">
+    <row r="1" spans="1:12" s="1" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>41</v>
       </c>
@@ -7569,7 +7592,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:12">
       <c r="A2" s="7" t="s">
         <v>42</v>
       </c>
@@ -7587,7 +7610,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:12">
       <c r="A3" s="7" t="s">
         <v>42</v>
       </c>
@@ -7605,7 +7628,7 @@
         <v>0.16170000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:12">
       <c r="A4" s="7" t="s">
         <v>42</v>
       </c>
@@ -7623,7 +7646,7 @@
         <v>25.18</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:12">
       <c r="A5" s="7" t="s">
         <v>42</v>
       </c>
@@ -7641,7 +7664,7 @@
         <v>1.4550000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:12">
       <c r="A6" s="7" t="s">
         <v>42</v>
       </c>
@@ -7659,7 +7682,7 @@
         <v>2.4571999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:12">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -7677,7 +7700,7 @@
         <v>-4.9639999999999997E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:12">
       <c r="A8" s="7" t="s">
         <v>42</v>
       </c>
@@ -7695,7 +7718,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:12">
       <c r="A9" s="7" t="s">
         <v>42</v>
       </c>
@@ -7728,7 +7751,7 @@
         <v>0.99521000000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="3" customFormat="1">
+    <row r="10" spans="1:12" s="3" customFormat="1">
       <c r="A10" s="7" t="s">
         <v>42</v>
       </c>
@@ -7748,12 +7771,14 @@
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
-      <c r="K10" s="22">
-        <f>K12/3900</f>
-        <v>7.6152769230769237E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="K10" s="13">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="7" t="s">
         <v>42</v>
       </c>
@@ -7771,7 +7796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:12">
       <c r="A12" s="7" t="s">
         <v>42</v>
       </c>
@@ -7807,7 +7832,7 @@
         <v>29.699580000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:12">
       <c r="A13" s="7" t="s">
         <v>54</v>
       </c>
@@ -7825,7 +7850,7 @@
         <v>calculated</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:12">
       <c r="A14" s="8" t="s">
         <v>44</v>
       </c>
@@ -7849,7 +7874,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:12">
       <c r="A15" s="7" t="s">
         <v>49</v>
       </c>
@@ -7867,7 +7892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:12">
       <c r="A16" s="7" t="s">
         <v>49</v>
       </c>
@@ -8025,7 +8050,7 @@
       <c r="J23" s="7">
         <v>7904</v>
       </c>
-      <c r="K23" s="23">
+      <c r="K23" s="22">
         <f>J23</f>
         <v>7904</v>
       </c>
@@ -8101,7 +8126,7 @@
       <c r="F26" s="7">
         <v>3.8497903160641202E-2</v>
       </c>
-      <c r="K26" s="23">
+      <c r="K26" s="22">
         <f>F26</f>
         <v>3.8497903160641202E-2</v>
       </c>
@@ -8182,7 +8207,7 @@
       <c r="F29" s="7">
         <v>8.9041257982607895</v>
       </c>
-      <c r="K29" s="23">
+      <c r="K29" s="22">
         <f>F29</f>
         <v>8.9041257982607895</v>
       </c>
@@ -8203,7 +8228,7 @@
       <c r="F30" s="7">
         <v>5.0806651342384201</v>
       </c>
-      <c r="K30" s="23">
+      <c r="K30" s="22">
         <f>F30</f>
         <v>5.0806651342384201</v>
       </c>
@@ -8240,8 +8265,10 @@
         <v>48.634430000000002</v>
       </c>
       <c r="K31" s="16">
-        <f>AVERAGE(I31:J31)</f>
-        <v>43.244515</v>
+        <v>64</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -8264,7 +8291,7 @@
       <c r="F32" s="7">
         <v>4.7282893919530899E-3</v>
       </c>
-      <c r="K32" s="23">
+      <c r="K32" s="22">
         <f>F32</f>
         <v>4.7282893919530899E-3</v>
       </c>
@@ -8283,7 +8310,7 @@
         <v>0.83999999999999897</v>
       </c>
       <c r="K33" s="2">
-        <f t="shared" ref="K32:K39" si="1">C33</f>
+        <f t="shared" ref="K33:K39" si="1">C33</f>
         <v>0.84</v>
       </c>
     </row>
@@ -8362,7 +8389,7 @@
       <c r="H37" s="7"/>
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
-      <c r="K37" s="23">
+      <c r="K37" s="22">
         <f>F37</f>
         <v>0.38994431160946502</v>
       </c>
@@ -8386,7 +8413,7 @@
       <c r="F38" s="7">
         <v>0.313929226152732</v>
       </c>
-      <c r="K38" s="23">
+      <c r="K38" s="22">
         <f>F38</f>
         <v>0.313929226152732</v>
       </c>
@@ -8470,11 +8497,11 @@
       <c r="F42" s="7">
         <v>0.27139278132733902</v>
       </c>
-      <c r="K42" s="23">
+      <c r="K42" s="22">
         <f>F42</f>
         <v>0.27139278132733902</v>
       </c>
-      <c r="L42" s="23" t="s">
+      <c r="L42" s="22" t="s">
         <v>103</v>
       </c>
     </row>
@@ -8554,7 +8581,7 @@
       <c r="F45" s="7">
         <v>0.67110777222439699</v>
       </c>
-      <c r="K45" s="23">
+      <c r="K45" s="22">
         <f>F45</f>
         <v>0.67110777222439699</v>
       </c>
@@ -8628,8 +8655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8643,7 +8670,7 @@
     <col min="11" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1">
+    <row r="1" spans="1:11" s="1" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>41</v>
       </c>
@@ -8675,7 +8702,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11">
       <c r="A2" s="7" t="s">
         <v>42</v>
       </c>
@@ -8693,7 +8720,7 @@
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11">
       <c r="A3" s="7" t="s">
         <v>42</v>
       </c>
@@ -8711,7 +8738,7 @@
         <v>0.23499999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:11">
       <c r="A4" s="7" t="s">
         <v>42</v>
       </c>
@@ -8729,7 +8756,7 @@
         <v>23.3874</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:11">
       <c r="A5" s="7" t="s">
         <v>42</v>
       </c>
@@ -8747,7 +8774,7 @@
         <v>1.7310000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11">
       <c r="A6" s="7" t="s">
         <v>42</v>
       </c>
@@ -8765,7 +8792,7 @@
         <v>2.2517999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:11">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -8783,7 +8810,7 @@
         <v>-5.4039999999999998E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:11">
       <c r="A8" s="7" t="s">
         <v>42</v>
       </c>
@@ -8801,7 +8828,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:11">
       <c r="A9" s="7" t="s">
         <v>42</v>
       </c>
@@ -8834,7 +8861,7 @@
         <v>0.99734</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="3" customFormat="1">
+    <row r="10" spans="1:11" s="3" customFormat="1">
       <c r="A10" s="7" t="s">
         <v>42</v>
       </c>
@@ -8853,12 +8880,14 @@
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
-      <c r="J10" s="22">
-        <f>J12/3900</f>
-        <v>1.0098825641025641E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="J10" s="13">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="7" t="s">
         <v>42</v>
       </c>
@@ -8876,7 +8905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:11">
       <c r="A12" s="7" t="s">
         <v>42</v>
       </c>
@@ -8909,7 +8938,7 @@
         <v>39.385420000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:11">
       <c r="A13" s="7" t="s">
         <v>54</v>
       </c>
@@ -8927,7 +8956,7 @@
         <v>calculated</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:11">
       <c r="A14" s="8" t="s">
         <v>44</v>
       </c>
@@ -8950,7 +8979,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:11">
       <c r="A15" s="7" t="s">
         <v>49</v>
       </c>
@@ -8968,7 +8997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:11">
       <c r="A16" s="7" t="s">
         <v>49</v>
       </c>
@@ -8987,7 +9016,7 @@
       <c r="F16" s="7">
         <v>20.230664535218999</v>
       </c>
-      <c r="J16" s="23">
+      <c r="J16" s="22">
         <f>F16</f>
         <v>20.230664535218999</v>
       </c>
@@ -9127,13 +9156,11 @@
       <c r="F23" s="7">
         <v>12338.9937966083</v>
       </c>
-      <c r="J23" s="23">
+      <c r="J23" s="22">
         <f>F23</f>
         <v>12338.9937966083</v>
       </c>
-      <c r="K23" s="4" t="s">
-        <v>101</v>
-      </c>
+      <c r="K23" s="4"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="11" t="s">
@@ -9288,7 +9315,7 @@
       <c r="F29" s="7">
         <v>5.7797041220733103</v>
       </c>
-      <c r="J29" s="23">
+      <c r="J29" s="22">
         <f>F29</f>
         <v>5.7797041220733103</v>
       </c>
@@ -9309,7 +9336,7 @@
       <c r="F30" s="7">
         <v>4.9405752650944903</v>
       </c>
-      <c r="J30" s="23">
+      <c r="J30" s="22">
         <f>F30</f>
         <v>4.9405752650944903</v>
       </c>
@@ -9367,7 +9394,7 @@
       <c r="F32" s="7">
         <v>4.3073313525717203E-3</v>
       </c>
-      <c r="J32" s="23">
+      <c r="J32" s="22">
         <f>F32</f>
         <v>4.3073313525717203E-3</v>
       </c>
@@ -9386,7 +9413,7 @@
         <v>0.83999999999999897</v>
       </c>
       <c r="J33" s="2">
-        <f t="shared" ref="J32:J39" si="1">C33</f>
+        <f t="shared" ref="J33:J39" si="1">C33</f>
         <v>0.84</v>
       </c>
     </row>
@@ -9464,7 +9491,7 @@
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
       <c r="I37" s="7"/>
-      <c r="J37" s="23">
+      <c r="J37" s="22">
         <f>F37</f>
         <v>0.400752854697557</v>
       </c>
@@ -9488,7 +9515,7 @@
       <c r="F38" s="7">
         <v>0.30899069780498301</v>
       </c>
-      <c r="J38" s="23">
+      <c r="J38" s="22">
         <f>F38</f>
         <v>0.30899069780498301</v>
       </c>
@@ -9573,11 +9600,11 @@
       <c r="F42" s="7">
         <v>0.355075216876657</v>
       </c>
-      <c r="J42" s="23">
+      <c r="J42" s="22">
         <f>F42</f>
         <v>0.355075216876657</v>
       </c>
-      <c r="K42" s="23"/>
+      <c r="K42" s="22"/>
     </row>
     <row r="43" spans="1:11">
       <c r="A43" s="7" t="s">
@@ -9652,7 +9679,7 @@
       <c r="F45" s="7">
         <v>0.69017285456830202</v>
       </c>
-      <c r="J45" s="23">
+      <c r="J45" s="22">
         <f>F45</f>
         <v>0.69017285456830202</v>
       </c>
@@ -11222,15 +11249,15 @@
       </c>
       <c r="H10" s="13">
         <f>'9 - Temp Early Hardwood'!K10</f>
-        <v>1.097478717948718E-2</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="I10" s="13">
         <f>'10 -  Mid Hardwood'!K10</f>
-        <v>7.6152769230769237E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="J10" s="13">
         <f>'11 - Late Hardwood'!J10</f>
-        <v>1.0098825641025641E-2</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -11594,11 +11621,11 @@
       </c>
       <c r="F23" s="14">
         <f>'8 - Late Conifer'!I23</f>
-        <v>1000</v>
+        <v>4426.9797352549103</v>
       </c>
       <c r="H23" s="14">
         <f>'9 - Temp Early Hardwood'!K23</f>
-        <v>10000</v>
+        <v>7904</v>
       </c>
       <c r="I23" s="14">
         <f>'10 -  Mid Hardwood'!K23</f>
@@ -11845,18 +11872,18 @@
       </c>
       <c r="F31" s="16">
         <f>'8 - Late Conifer'!I31</f>
-        <v>72.380390000000006</v>
+        <v>50</v>
       </c>
       <c r="G31" s="19">
         <v>63.96669</v>
       </c>
       <c r="H31" s="2">
         <f>'9 - Temp Early Hardwood'!K31</f>
-        <v>56.31326</v>
+        <v>57.3</v>
       </c>
       <c r="I31" s="16">
         <f>'10 -  Mid Hardwood'!K31</f>
-        <v>43.244515</v>
+        <v>64</v>
       </c>
       <c r="J31" s="16">
         <f>'11 - Late Hardwood'!J31</f>

</xml_diff>